<commit_message>
updating function for uploading new product catalog
</commit_message>
<xml_diff>
--- a/PREP REQ - TEMPLATE.xlsx
+++ b/PREP REQ - TEMPLATE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcuvin/purveyor_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C96E6A8-90A4-BB41-8C0C-111DABAD9B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF164FD-175B-964E-9596-880A5257465B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="29940" windowHeight="17600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +113,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
+        <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
@@ -181,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -226,6 +232,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2753,7 +2765,7 @@
   <dimension ref="A1:V987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2793,22 +2805,22 @@
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="3"/>

</xml_diff>